<commit_message>
Update opentrons version to 7.3.0 in requirements.txt and the excel file example.
</commit_message>
<xml_diff>
--- a/protocol_setup/protocol_setup.xlsx
+++ b/protocol_setup/protocol_setup.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roger\Documents\programas\opentrons_tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roger\Documents\programas\opentrons_tests\Opentrons_LARP_protocol_generator\protocol_setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0EE74E-FE94-4F3F-A7D3-0E07F8389ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3FBB05-1820-4584-9631-F7D55492B520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="18159" windowHeight="9585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -940,8 +940,8 @@
   </sheetPr>
   <dimension ref="A1:V140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q43" sqref="Q43"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1674,7 +1674,7 @@
         <v>41</v>
       </c>
       <c r="C33" s="3">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>12</v>
@@ -1708,7 +1708,7 @@
         <v>42</v>
       </c>
       <c r="C34" s="3">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
new calibration, updated also on xlsx, speed to default now.
</commit_message>
<xml_diff>
--- a/protocol_setup/protocol_setup.xlsx
+++ b/protocol_setup/protocol_setup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roger\Documents\programas\opentrons_tests\Opentrons_LARP_protocol_generator\protocol_setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3FBB05-1820-4584-9631-F7D55492B520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C56012-A7F0-452A-838A-578AC94C1C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="18159" windowHeight="9585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,9 +40,6 @@
     <t>lamaiufrgscinza_12_tuberack_20000ul</t>
   </si>
   <si>
-    <t>lamaiufrgsbranco_re_12_tuberack_15000ul</t>
-  </si>
-  <si>
     <t>MAX VOLUME</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>C4</t>
   </si>
   <si>
-    <t>lamaiufrgspreto24_re_24_tuberack_5000ul</t>
-  </si>
-  <si>
     <t>A5</t>
   </si>
   <si>
@@ -197,6 +191,12 @@
   </si>
   <si>
     <t>5 A3</t>
+  </si>
+  <si>
+    <t>lamaiufrgsbranco_re2_12_tuberack_15000ul</t>
+  </si>
+  <si>
+    <t>lamaiufrgspreto24_re2_24_tuberack_5000ul</t>
   </si>
 </sst>
 </file>
@@ -940,8 +940,8 @@
   </sheetPr>
   <dimension ref="A1:V140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N59" sqref="N59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -982,7 +982,7 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="M2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
@@ -1004,7 +1004,7 @@
         <v>4</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="I3" s="1"/>
       <c r="M3" s="1" t="s">
@@ -1024,28 +1024,28 @@
     </row>
     <row r="4" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
         <v>20000</v>
       </c>
       <c r="C4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H4" s="1">
         <v>15000</v>
       </c>
       <c r="I4" s="1"/>
       <c r="M4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N4" s="1">
         <v>20000</v>
       </c>
       <c r="O4" s="1"/>
       <c r="T4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U4" s="1">
         <v>20000</v>
@@ -1054,28 +1054,28 @@
     </row>
     <row r="5" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1">
         <v>7</v>
       </c>
       <c r="C5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H5" s="1">
         <v>5</v>
       </c>
       <c r="I5" s="1"/>
       <c r="M5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N5" s="1">
         <v>9</v>
       </c>
       <c r="O5" s="1"/>
       <c r="T5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U5" s="1">
         <v>9</v>
@@ -1084,80 +1084,80 @@
     </row>
     <row r="6" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="U6" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="G7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="M7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="T7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U7" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8" s="3">
         <v>10000</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O8" s="3">
         <v>10000</v>
       </c>
       <c r="T8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U8" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="U8" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="V8" s="3">
         <v>300</v>
@@ -1165,37 +1165,37 @@
     </row>
     <row r="9" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" s="3">
         <v>10000</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="M9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O9" s="3">
         <v>10000</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U9" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V9" s="3">
         <v>300</v>
@@ -1203,248 +1203,248 @@
     </row>
     <row r="10" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" s="3">
         <v>10000</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="T10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
     </row>
     <row r="11" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="3">
         <v>10000</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="T11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
     </row>
     <row r="12" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="G12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="T12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
     </row>
     <row r="13" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="G13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="T13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
     </row>
     <row r="14" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="G14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="T14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
     </row>
     <row r="15" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="G15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="M15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="T15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
     </row>
     <row r="16" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="G16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="M16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="T16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
     </row>
     <row r="17" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="G17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="M17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="T17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
     </row>
     <row r="18" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="G18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="M18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="T18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
     </row>
     <row r="19" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="G19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="M19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="T19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
@@ -1538,55 +1538,55 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="C28" s="1"/>
       <c r="G28" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="I28" s="1"/>
       <c r="M28" s="1" t="s">
         <v>4</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="O28" s="1"/>
       <c r="T28" s="1" t="s">
         <v>4</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="V28" s="1"/>
     </row>
     <row r="29" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29" s="1">
         <v>15000</v>
       </c>
       <c r="C29" s="1"/>
       <c r="G29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H29" s="1">
         <v>15000</v>
       </c>
       <c r="I29" s="1"/>
       <c r="M29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N29" s="1">
         <v>5000</v>
       </c>
       <c r="O29" s="1"/>
       <c r="T29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U29" s="1">
         <v>5000</v>
@@ -1595,28 +1595,28 @@
     </row>
     <row r="30" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30" s="1">
         <v>4</v>
       </c>
       <c r="C30" s="1"/>
       <c r="G30" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H30" s="1">
         <v>2</v>
       </c>
       <c r="I30" s="1"/>
       <c r="M30" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N30" s="1">
         <v>6</v>
       </c>
       <c r="O30" s="1"/>
       <c r="T30" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U30" s="1">
         <v>6</v>
@@ -1625,76 +1625,76 @@
     </row>
     <row r="31" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="U31" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="G32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I32" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="M32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N32" s="1" t="s">
+      <c r="O32" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O32" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="T32" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U32" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="V32" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C33" s="3">
         <v>10000</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="M33" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N33" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="T33" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="U33" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="V33" s="3">
         <v>300</v>
@@ -1702,33 +1702,33 @@
     </row>
     <row r="34" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C34" s="3">
         <v>10000</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="M34" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="T34" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U34" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="V34" s="3">
         <v>300</v>
@@ -1736,29 +1736,29 @@
     </row>
     <row r="35" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="G35" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="M35" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N35" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O35" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U35" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="V35" s="3">
         <v>300</v>
@@ -1766,29 +1766,29 @@
     </row>
     <row r="36" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="G36" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="M36" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="T36" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U36" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="V36" s="3">
         <v>300</v>
@@ -1796,180 +1796,180 @@
     </row>
     <row r="37" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="G37" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="M37" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N37" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="U37" s="3"/>
       <c r="V37" s="3"/>
     </row>
     <row r="38" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="G38" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
       <c r="M38" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="T38" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="U38" s="3"/>
       <c r="V38" s="3"/>
     </row>
     <row r="39" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="G39" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
       <c r="M39" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
       <c r="T39" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U39" s="3"/>
       <c r="V39" s="3"/>
     </row>
     <row r="40" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="G40" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
       <c r="M40" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
       <c r="T40" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U40" s="3"/>
       <c r="V40" s="3"/>
     </row>
     <row r="41" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="G41" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
       <c r="M41" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
       <c r="T41" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U41" s="3"/>
       <c r="V41" s="3"/>
     </row>
     <row r="42" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="G42" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
       <c r="M42" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
       <c r="T42" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="U42" s="3"/>
       <c r="V42" s="3"/>
     </row>
     <row r="43" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="G43" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="M43" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
       <c r="T43" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="U43" s="3"/>
       <c r="V43" s="3"/>
     </row>
     <row r="44" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="G44" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
       <c r="M44" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
       <c r="T44" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="U44" s="3"/>
       <c r="V44" s="3"/>
@@ -1982,12 +1982,12 @@
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="M45" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
       <c r="T45" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U45" s="3"/>
       <c r="V45" s="3"/>
@@ -2000,12 +2000,12 @@
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="M46" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
       <c r="T46" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U46" s="3"/>
       <c r="V46" s="3"/>
@@ -2018,12 +2018,12 @@
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="M47" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N47" s="3"/>
       <c r="O47" s="3"/>
       <c r="T47" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U47" s="3"/>
       <c r="V47" s="3"/>
@@ -2036,12 +2036,12 @@
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="M48" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
       <c r="T48" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U48" s="3"/>
       <c r="V48" s="3"/>
@@ -2054,12 +2054,12 @@
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="M49" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N49" s="3"/>
       <c r="O49" s="3"/>
       <c r="T49" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U49" s="3"/>
       <c r="V49" s="3"/>
@@ -2072,48 +2072,48 @@
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
       <c r="M50" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
       <c r="T50" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U50" s="3"/>
       <c r="V50" s="3"/>
     </row>
     <row r="51" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="M51" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
       <c r="T51" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="U51" s="3"/>
       <c r="V51" s="3"/>
     </row>
     <row r="52" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="M52" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N52" s="3"/>
       <c r="O52" s="3"/>
       <c r="T52" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="U52" s="3"/>
       <c r="V52" s="3"/>
     </row>
     <row r="53" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="M53" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
       <c r="T53" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="U53" s="3"/>
       <c r="V53" s="3"/>
@@ -2123,54 +2123,54 @@
         <v>4</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C54" s="1"/>
       <c r="M54" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N54" s="3"/>
       <c r="O54" s="3"/>
       <c r="T54" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="U54" s="3"/>
       <c r="V54" s="3"/>
     </row>
     <row r="55" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B55" s="1">
         <v>20000</v>
       </c>
       <c r="C55" s="1"/>
       <c r="M55" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N55" s="3"/>
       <c r="O55" s="3"/>
       <c r="T55" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="U55" s="3"/>
       <c r="V55" s="3"/>
     </row>
     <row r="56" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B56" s="1">
         <v>1</v>
       </c>
       <c r="C56" s="1"/>
       <c r="M56" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="N56" s="3"/>
       <c r="O56" s="3"/>
       <c r="T56" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="U56" s="3"/>
       <c r="V56" s="3"/>
@@ -2180,22 +2180,22 @@
     </row>
     <row r="58" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="M58" s="4"/>
     </row>
     <row r="59" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C59" s="3">
         <v>80000</v>
@@ -2204,14 +2204,14 @@
         <v>4</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="O59" s="1"/>
       <c r="T59" s="1" t="s">
         <v>4</v>
       </c>
       <c r="U59" s="1" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="V59" s="1"/>
     </row>
@@ -2220,14 +2220,14 @@
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="M60" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N60" s="1">
         <v>5000</v>
       </c>
       <c r="O60" s="1"/>
       <c r="T60" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U60" s="1">
         <v>5000</v>
@@ -2239,14 +2239,14 @@
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="M61" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N61" s="1">
         <v>3</v>
       </c>
       <c r="O61" s="1"/>
       <c r="T61" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U61" s="1">
         <v>3</v>
@@ -2258,7 +2258,7 @@
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="U62" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
@@ -2266,22 +2266,22 @@
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="M63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N63" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N63" s="1" t="s">
+      <c r="O63" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O63" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="T63" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U63" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="V63" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
@@ -2289,12 +2289,12 @@
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="M64" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N64" s="3"/>
       <c r="O64" s="3"/>
       <c r="T64" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="U64" s="3"/>
       <c r="V64" s="3"/>
@@ -2304,12 +2304,12 @@
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="M65" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N65" s="3"/>
       <c r="O65" s="3"/>
       <c r="T65" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U65" s="3"/>
       <c r="V65" s="3"/>
@@ -2319,12 +2319,12 @@
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="M66" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N66" s="3"/>
       <c r="O66" s="3"/>
       <c r="T66" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U66" s="3"/>
       <c r="V66" s="3"/>
@@ -2334,12 +2334,12 @@
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="M67" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N67" s="3"/>
       <c r="O67" s="3"/>
       <c r="T67" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U67" s="3"/>
       <c r="V67" s="3"/>
@@ -2349,12 +2349,12 @@
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="M68" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N68" s="3"/>
       <c r="O68" s="3"/>
       <c r="T68" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="U68" s="3"/>
       <c r="V68" s="3"/>
@@ -2364,12 +2364,12 @@
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="M69" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N69" s="3"/>
       <c r="O69" s="3"/>
       <c r="T69" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="U69" s="3"/>
       <c r="V69" s="3"/>
@@ -2379,12 +2379,12 @@
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="M70" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N70" s="3"/>
       <c r="O70" s="3"/>
       <c r="T70" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U70" s="3"/>
       <c r="V70" s="3"/>
@@ -2394,12 +2394,12 @@
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="M71" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N71" s="3"/>
       <c r="O71" s="3"/>
       <c r="T71" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U71" s="3"/>
       <c r="V71" s="3"/>
@@ -2409,12 +2409,12 @@
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="M72" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N72" s="3"/>
       <c r="O72" s="3"/>
       <c r="T72" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U72" s="3"/>
       <c r="V72" s="3"/>
@@ -2424,12 +2424,12 @@
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="M73" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N73" s="3"/>
       <c r="O73" s="3"/>
       <c r="T73" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="U73" s="3"/>
       <c r="V73" s="3"/>
@@ -2439,12 +2439,12 @@
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="M74" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N74" s="3"/>
       <c r="O74" s="3"/>
       <c r="T74" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="U74" s="3"/>
       <c r="V74" s="3"/>
@@ -2454,12 +2454,12 @@
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="M75" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N75" s="3"/>
       <c r="O75" s="3"/>
       <c r="T75" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="U75" s="3"/>
       <c r="V75" s="3"/>
@@ -2469,144 +2469,144 @@
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="M76" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N76" s="3"/>
       <c r="O76" s="3"/>
       <c r="T76" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U76" s="3"/>
       <c r="V76" s="3"/>
     </row>
     <row r="77" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="M77" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N77" s="3"/>
       <c r="O77" s="3"/>
       <c r="T77" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U77" s="3"/>
       <c r="V77" s="3"/>
     </row>
     <row r="78" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="M78" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N78" s="3"/>
       <c r="O78" s="3"/>
       <c r="T78" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U78" s="3"/>
       <c r="V78" s="3"/>
     </row>
     <row r="79" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="M79" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N79" s="3"/>
       <c r="O79" s="3"/>
       <c r="T79" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U79" s="3"/>
       <c r="V79" s="3"/>
     </row>
     <row r="80" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="M80" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N80" s="3"/>
       <c r="O80" s="3"/>
       <c r="T80" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U80" s="3"/>
       <c r="V80" s="3"/>
     </row>
     <row r="81" spans="13:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="M81" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N81" s="3"/>
       <c r="O81" s="3"/>
       <c r="T81" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U81" s="3"/>
       <c r="V81" s="3"/>
     </row>
     <row r="82" spans="13:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="M82" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N82" s="3"/>
       <c r="O82" s="3"/>
       <c r="T82" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="U82" s="3"/>
       <c r="V82" s="3"/>
     </row>
     <row r="83" spans="13:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="M83" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N83" s="3"/>
       <c r="O83" s="3"/>
       <c r="T83" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="U83" s="3"/>
       <c r="V83" s="3"/>
     </row>
     <row r="84" spans="13:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="M84" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N84" s="3"/>
       <c r="O84" s="3"/>
       <c r="T84" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="U84" s="3"/>
       <c r="V84" s="3"/>
     </row>
     <row r="85" spans="13:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="M85" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N85" s="3"/>
       <c r="O85" s="3"/>
       <c r="T85" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="U85" s="3"/>
       <c r="V85" s="3"/>
     </row>
     <row r="86" spans="13:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="M86" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N86" s="3"/>
       <c r="O86" s="3"/>
       <c r="T86" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="U86" s="3"/>
       <c r="V86" s="3"/>
     </row>
     <row r="87" spans="13:22" ht="12.65" x14ac:dyDescent="0.3">
       <c r="M87" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="N87" s="3"/>
       <c r="O87" s="3"/>
       <c r="T87" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="U87" s="3"/>
       <c r="V87" s="3"/>

</xml_diff>

<commit_message>
update again protocol_setup and the xslx_to_protocol
</commit_message>
<xml_diff>
--- a/protocol_setup/protocol_setup.xlsx
+++ b/protocol_setup/protocol_setup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roger\Documents\programas\opentrons_tests\Opentrons_LARP_protocol_generator\protocol_setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C56012-A7F0-452A-838A-578AC94C1C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB685B9-FE07-4D8F-A61A-589C825AE88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="18159" windowHeight="9585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,18 +215,21 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -253,6 +256,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -940,8 +944,8 @@
   </sheetPr>
   <dimension ref="A1:V140"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N59" sqref="N59"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2142,7 +2146,7 @@
         <v>6</v>
       </c>
       <c r="B55" s="1">
-        <v>20000</v>
+        <v>100000</v>
       </c>
       <c r="C55" s="1"/>
       <c r="M55" s="1" t="s">

</xml_diff>

<commit_message>
modifications in the default protocol setup to be clearer and script to avoid error after generation of graphical protocol
</commit_message>
<xml_diff>
--- a/protocol_setup/protocol_setup.xlsx
+++ b/protocol_setup/protocol_setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roger\Documents\programas\opentrons_tests\Opentrons_LARP_protocol_generator\protocol_setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB685B9-FE07-4D8F-A61A-589C825AE88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E38D2B-BB2A-4DB0-859B-437DE48516FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="18159" windowHeight="9585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="59">
-  <si>
-    <t>SHEET TO SETUP LARP SYNTHESIS</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="62">
   <si>
     <t>PRECURSORS AND LIGANDS</t>
   </si>
@@ -197,13 +194,25 @@
   </si>
   <si>
     <t>lamaiufrgspreto24_re2_24_tuberack_5000ul</t>
+  </si>
+  <si>
+    <t>THIS IS THE INTERMEDIATE PHASE, SET THE PRECURSOR SOLUTIONS AND ANTISOLVENTS</t>
+  </si>
+  <si>
+    <t>NOW YOU SET THE INJECTIONS FROM THE INTERMEDIATE TO THE ANTISOLVENT</t>
+  </si>
+  <si>
+    <t>INJECTIONS MUST CORRESPOND TO EACH OF THE ANTISOLVENT WELLS!!!</t>
+  </si>
+  <si>
+    <t>SHEET TO SETUP LARP SYNTHESIS _ SET THE PRECURSOR SOLUTIONS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -259,8 +268,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,6 +322,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -310,12 +359,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -324,7 +372,22 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -349,9 +412,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>5937</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>24369</xdr:rowOff>
+      <xdr:colOff>184067</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>41334</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2752725" cy="2667000"/>
     <xdr:pic>
@@ -373,7 +436,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4177145" y="217344"/>
+          <a:off x="4348913" y="431523"/>
           <a:ext cx="2752725" cy="2667000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -387,9 +450,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:colOff>480227</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>20851</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2752725" cy="2419350"/>
     <xdr:pic>
@@ -410,6 +473,10 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22865214" y="309252"/>
+          <a:ext cx="2752725" cy="2419350"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -459,11 +526,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>42059</xdr:colOff>
+      <xdr:colOff>567965</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>1113</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2609850" cy="2730211"/>
+    <xdr:ext cx="2867395" cy="2730211"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="6" name="image4.png" title="Image">
@@ -483,8 +550,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20794189" y="194088"/>
-          <a:ext cx="2609850" cy="2730211"/>
+          <a:off x="30773702" y="289514"/>
+          <a:ext cx="2867395" cy="2730211"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -494,249 +561,194 @@
     </xdr:pic>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>77190</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>71252</xdr:rowOff>
+      <xdr:colOff>237507</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>84823</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>142504</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>95003</xdr:rowOff>
+      <xdr:colOff>619213</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>101788</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1026" name="image1.png">
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Arrow: Left-Right 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6D3E09D-7E86-C8D5-DCA1-C67E1CD3D7A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A15FF3A-098E-C015-B24E-EEB68BB2C05F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="22474052" y="463138"/>
-          <a:ext cx="2772888" cy="2571007"/>
+          <a:off x="22622494" y="11273076"/>
+          <a:ext cx="3079102" cy="1467451"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom prst="leftRightArrow">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
       </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="LID4096" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>77190</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>71252</xdr:rowOff>
+      <xdr:colOff>415636</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>76341</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>142504</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>95003</xdr:rowOff>
+      <xdr:colOff>704036</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>93306</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1027" name="Picture 3">
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Arrow: Left-Right 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{426BF25B-FCFD-17DB-0183-23FD2AFD3F59}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8545BAF-12D5-4252-8B7B-5F2B94878DF3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="22474052" y="463138"/>
-          <a:ext cx="2772888" cy="2571007"/>
+          <a:off x="22800623" y="6718041"/>
+          <a:ext cx="2985796" cy="1467451"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom prst="leftRightArrow">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
       </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="LID4096" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>95003</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>184068</xdr:rowOff>
+      <xdr:colOff>364742</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>101790</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>142504</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>47501</xdr:rowOff>
+      <xdr:colOff>721001</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>16966</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1028" name="Picture 4">
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Arrow: Left-Right 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0C35EDC-FEE4-1DC4-05C7-1B9ECEE65B44}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5974148-2C49-4D34-BF1F-5A067D8A594B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="22491865" y="380010"/>
-          <a:ext cx="2755075" cy="2410691"/>
+          <a:off x="22749729" y="2833114"/>
+          <a:ext cx="3053655" cy="1467451"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom prst="leftRightArrow">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
       </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>95003</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>184068</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>142504</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>47501</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1029" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74326752-5A0C-A5A0-E33A-A788AC01EA6C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="22491865" y="380010"/>
-          <a:ext cx="2755075" cy="2410691"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="LID4096" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
@@ -942,10 +954,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V140"/>
+  <dimension ref="A1:Y140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -963,1669 +975,3047 @@
     <col min="15" max="15" width="23.6640625" customWidth="1"/>
     <col min="20" max="20" width="17.08203125" customWidth="1"/>
     <col min="21" max="21" width="29.5" customWidth="1"/>
+    <col min="24" max="24" width="15.9140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:25" ht="22.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="14"/>
+    </row>
+    <row r="2" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-    </row>
-    <row r="2" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="M2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="T2" s="11" t="s">
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+    </row>
+    <row r="3" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-    </row>
-    <row r="3" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V3" s="1"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+    </row>
+    <row r="4" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="G3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="M3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O3" s="1"/>
-      <c r="T3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="V3" s="1"/>
-    </row>
-    <row r="4" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="B4" s="1">
         <v>20000</v>
       </c>
       <c r="C4" s="1"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="13"/>
       <c r="G4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H4" s="1">
         <v>15000</v>
       </c>
       <c r="I4" s="1"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
       <c r="M4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N4" s="1">
         <v>20000</v>
       </c>
       <c r="O4" s="1"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
       <c r="T4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U4" s="1">
         <v>20000</v>
       </c>
       <c r="V4" s="1"/>
-    </row>
-    <row r="5" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+    </row>
+    <row r="5" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>7</v>
       </c>
       <c r="C5" s="1"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13"/>
       <c r="G5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H5" s="1">
         <v>5</v>
       </c>
       <c r="I5" s="1"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
       <c r="M5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N5" s="1">
         <v>9</v>
       </c>
       <c r="O5" s="1"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
       <c r="T5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U5" s="1">
         <v>9</v>
       </c>
       <c r="V5" s="1"/>
-    </row>
-    <row r="6" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="U6" s="9" t="s">
+      <c r="W5" s="14"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+    </row>
+    <row r="6" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+    </row>
+    <row r="7" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U7" s="9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="V7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="W7" s="14"/>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="14"/>
+    </row>
+    <row r="8" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="U7" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="3">
         <v>10000</v>
       </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
       <c r="M8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O8" s="3">
         <v>10000</v>
       </c>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
       <c r="T8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U8" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="U8" s="6" t="s">
-        <v>12</v>
       </c>
       <c r="V8" s="3">
         <v>300</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+    </row>
+    <row r="9" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="3">
         <v>10000</v>
       </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="13"/>
       <c r="G9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
       <c r="M9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O9" s="3">
         <v>10000</v>
       </c>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
       <c r="T9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U9" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="U9" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="V9" s="3">
         <v>300</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W9" s="14"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+    </row>
+    <row r="10" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3">
         <v>10000</v>
       </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>47</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
       <c r="M10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
       <c r="T10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
-    </row>
-    <row r="11" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W10" s="14"/>
+      <c r="X10" s="14"/>
+      <c r="Y10" s="14"/>
+    </row>
+    <row r="11" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="3">
         <v>10000</v>
       </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
       <c r="M11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
       <c r="T11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
-    </row>
-    <row r="12" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W11" s="14"/>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+    </row>
+    <row r="12" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>48</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
       <c r="M12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
       <c r="T12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
-    </row>
-    <row r="13" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14"/>
+    </row>
+    <row r="13" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>49</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
       <c r="M13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
       <c r="T13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
-    </row>
-    <row r="14" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W13" s="14"/>
+      <c r="X13" s="14"/>
+      <c r="Y13" s="14"/>
+    </row>
+    <row r="14" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>50</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
       <c r="M14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
       <c r="T14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
-    </row>
-    <row r="15" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
+    </row>
+    <row r="15" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
       <c r="M15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
       <c r="T15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
-    </row>
-    <row r="16" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
+      <c r="Y15" s="14"/>
+    </row>
+    <row r="16" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="13"/>
       <c r="G16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
       <c r="M16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
       <c r="T16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
-    </row>
-    <row r="17" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W16" s="14"/>
+      <c r="X16" s="14"/>
+      <c r="Y16" s="14"/>
+    </row>
+    <row r="17" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="13"/>
       <c r="G17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
       <c r="M17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
       <c r="T17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
-    </row>
-    <row r="18" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W17" s="14"/>
+      <c r="X17" s="14"/>
+      <c r="Y17" s="14"/>
+    </row>
+    <row r="18" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="13"/>
       <c r="G18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
       <c r="M18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
       <c r="T18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
-    </row>
-    <row r="19" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W18" s="14"/>
+      <c r="X18" s="14"/>
+      <c r="Y18" s="14"/>
+    </row>
+    <row r="19" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="13"/>
       <c r="G19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
       <c r="M19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
       <c r="T19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
-    </row>
-    <row r="20" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W19" s="14"/>
+      <c r="X19" s="14"/>
+      <c r="Y19" s="14"/>
+    </row>
+    <row r="20" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="13"/>
       <c r="G20" s="1"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
       <c r="M20" s="1"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
       <c r="T20" s="1"/>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
-    </row>
-    <row r="21" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W20" s="14"/>
+      <c r="X20" s="14"/>
+      <c r="Y20" s="14"/>
+    </row>
+    <row r="21" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="13"/>
       <c r="G21" s="1"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
       <c r="M21" s="1"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
       <c r="T21" s="1"/>
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
-    </row>
-    <row r="22" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W21" s="14"/>
+      <c r="X21" s="14"/>
+      <c r="Y21" s="14"/>
+    </row>
+    <row r="22" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="13"/>
       <c r="G22" s="2"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
       <c r="M22" s="2"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
       <c r="T22" s="2"/>
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
-    </row>
-    <row r="23" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W22" s="14"/>
+      <c r="X22" s="14"/>
+      <c r="Y22" s="14"/>
+    </row>
+    <row r="23" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="13"/>
       <c r="G23" s="2"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
       <c r="M23" s="2"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
       <c r="T23" s="2"/>
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
-    </row>
-    <row r="24" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W23" s="14"/>
+      <c r="X23" s="14"/>
+      <c r="Y23" s="14"/>
+    </row>
+    <row r="24" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="13"/>
       <c r="G24" s="1"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
       <c r="M24" s="1"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="14"/>
       <c r="T24" s="1"/>
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
-    </row>
-    <row r="25" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W24" s="14"/>
+      <c r="X24" s="14"/>
+      <c r="Y24" s="14"/>
+    </row>
+    <row r="25" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="13"/>
       <c r="G25" s="1"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
       <c r="M25" s="1"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="R25" s="18"/>
+      <c r="S25" s="14"/>
       <c r="T25" s="1"/>
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
-    </row>
-    <row r="28" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W25" s="14"/>
+      <c r="X25" s="14"/>
+      <c r="Y25" s="14"/>
+    </row>
+    <row r="26" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="14"/>
+      <c r="T26" s="14"/>
+      <c r="U26" s="14"/>
+      <c r="V26" s="14"/>
+      <c r="W26" s="14"/>
+      <c r="X26" s="14"/>
+      <c r="Y26" s="14"/>
+    </row>
+    <row r="27" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="14"/>
+      <c r="T27" s="14"/>
+      <c r="U27" s="14"/>
+      <c r="V27" s="14"/>
+      <c r="W27" s="14"/>
+      <c r="X27" s="14"/>
+      <c r="Y27" s="14"/>
+    </row>
+    <row r="28" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N28" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="G28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H28" s="1" t="s">
+      <c r="O28" s="1"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="14"/>
+      <c r="T28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U28" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I28" s="1"/>
-      <c r="M28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O28" s="1"/>
-      <c r="T28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U28" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="V28" s="1"/>
-    </row>
-    <row r="29" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W28" s="14"/>
+      <c r="X28" s="14"/>
+      <c r="Y28" s="14"/>
+    </row>
+    <row r="29" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B29" s="1">
         <v>15000</v>
       </c>
       <c r="C29" s="1"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="13"/>
       <c r="G29" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H29" s="1">
         <v>15000</v>
       </c>
       <c r="I29" s="1"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
       <c r="M29" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N29" s="1">
         <v>5000</v>
       </c>
       <c r="O29" s="1"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18"/>
+      <c r="S29" s="14"/>
       <c r="T29" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U29" s="1">
         <v>5000</v>
       </c>
       <c r="V29" s="1"/>
-    </row>
-    <row r="30" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W29" s="14"/>
+      <c r="X29" s="14"/>
+      <c r="Y29" s="14"/>
+    </row>
+    <row r="30" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30" s="1">
         <v>4</v>
       </c>
       <c r="C30" s="1"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="13"/>
       <c r="G30" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H30" s="1">
         <v>2</v>
       </c>
       <c r="I30" s="1"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
       <c r="M30" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N30" s="1">
         <v>6</v>
       </c>
       <c r="O30" s="1"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="14"/>
       <c r="T30" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U30" s="1">
         <v>6</v>
       </c>
       <c r="V30" s="1"/>
-    </row>
-    <row r="31" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="U31" s="9" t="s">
+      <c r="W30" s="14"/>
+      <c r="X30" s="14"/>
+      <c r="Y30" s="14"/>
+    </row>
+    <row r="31" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="R31" s="18"/>
+      <c r="S31" s="14"/>
+      <c r="T31" s="14"/>
+      <c r="U31" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="V31" s="14"/>
+      <c r="W31" s="14"/>
+      <c r="X31" s="14"/>
+      <c r="Y31" s="14"/>
+    </row>
+    <row r="32" spans="1:25" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="14"/>
+      <c r="T32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U32" s="9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="32" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="1" t="s">
+      <c r="V32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="W32" s="14"/>
+      <c r="X32" s="14"/>
+      <c r="Y32" s="14"/>
+    </row>
+    <row r="33" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="T32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="U32" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="V32" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="B33" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" s="3">
         <v>10000</v>
       </c>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="13"/>
       <c r="G33" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
       <c r="M33" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N33" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="O33" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O33" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="14"/>
       <c r="T33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="U33" s="6" t="s">
-        <v>55</v>
+        <v>10</v>
+      </c>
+      <c r="U33" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="V33" s="3">
         <v>300</v>
       </c>
-    </row>
-    <row r="34" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W33" s="14"/>
+      <c r="X33" s="14"/>
+      <c r="Y33" s="14"/>
+    </row>
+    <row r="34" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34" s="3">
         <v>10000</v>
       </c>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="13"/>
       <c r="G34" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
       <c r="M34" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N34" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="O34" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O34" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="14"/>
       <c r="T34" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U34" s="6" t="s">
-        <v>55</v>
+        <v>12</v>
+      </c>
+      <c r="U34" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="V34" s="3">
         <v>300</v>
       </c>
-    </row>
-    <row r="35" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W34" s="14"/>
+      <c r="X34" s="14"/>
+      <c r="Y34" s="14"/>
+    </row>
+    <row r="35" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="13"/>
       <c r="G35" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
       <c r="M35" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="O35" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O35" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="14"/>
       <c r="T35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="U35" s="6" t="s">
-        <v>56</v>
+        <v>13</v>
+      </c>
+      <c r="U35" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="V35" s="3">
         <v>300</v>
       </c>
-    </row>
-    <row r="36" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W35" s="14"/>
+      <c r="X35" s="14"/>
+      <c r="Y35" s="14"/>
+    </row>
+    <row r="36" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="13"/>
       <c r="G36" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
       <c r="M36" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="O36" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O36" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="14"/>
       <c r="T36" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="U36" s="6" t="s">
-        <v>56</v>
+        <v>14</v>
+      </c>
+      <c r="U36" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="V36" s="3">
         <v>300</v>
       </c>
-    </row>
-    <row r="37" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W36" s="14"/>
+      <c r="X36" s="14"/>
+      <c r="Y36" s="14"/>
+    </row>
+    <row r="37" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="13"/>
       <c r="G37" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
       <c r="M37" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N37" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="O37" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O37" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="P37" s="13"/>
+      <c r="Q37" s="13"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
       <c r="T37" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="U37" s="3"/>
-      <c r="V37" s="3"/>
-    </row>
-    <row r="38" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="U37" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="V37" s="3">
+        <v>300</v>
+      </c>
+      <c r="W37" s="14"/>
+      <c r="X37" s="14"/>
+      <c r="Y37" s="14"/>
+    </row>
+    <row r="38" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="13"/>
       <c r="G38" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
       <c r="M38" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
       <c r="T38" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="U38" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="U38" s="5"/>
       <c r="V38" s="3"/>
-    </row>
-    <row r="39" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W38" s="14"/>
+      <c r="X38" s="14"/>
+      <c r="Y38" s="14"/>
+    </row>
+    <row r="39" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="13"/>
       <c r="G39" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
       <c r="M39" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
+      <c r="P39" s="13"/>
+      <c r="Q39" s="13"/>
+      <c r="R39" s="14"/>
+      <c r="S39" s="14"/>
       <c r="T39" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U39" s="3"/>
       <c r="V39" s="3"/>
-    </row>
-    <row r="40" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W39" s="14"/>
+      <c r="X39" s="14"/>
+      <c r="Y39" s="14"/>
+    </row>
+    <row r="40" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="13"/>
       <c r="G40" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
       <c r="M40" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
+      <c r="P40" s="13"/>
+      <c r="Q40" s="13"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
       <c r="T40" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U40" s="3"/>
       <c r="V40" s="3"/>
-    </row>
-    <row r="41" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W40" s="14"/>
+      <c r="X40" s="14"/>
+      <c r="Y40" s="14"/>
+    </row>
+    <row r="41" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="13"/>
       <c r="G41" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
       <c r="M41" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="14"/>
+      <c r="S41" s="14"/>
       <c r="T41" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U41" s="3"/>
       <c r="V41" s="3"/>
-    </row>
-    <row r="42" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W41" s="14"/>
+      <c r="X41" s="14"/>
+      <c r="Y41" s="14"/>
+    </row>
+    <row r="42" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="13"/>
       <c r="G42" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
       <c r="M42" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
+      <c r="P42" s="13"/>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
       <c r="T42" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U42" s="3"/>
       <c r="V42" s="3"/>
-    </row>
-    <row r="43" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W42" s="14"/>
+      <c r="X42" s="14"/>
+      <c r="Y42" s="14"/>
+    </row>
+    <row r="43" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="13"/>
       <c r="G43" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
       <c r="M43" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
+      <c r="P43" s="13"/>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="14"/>
+      <c r="S43" s="14"/>
       <c r="T43" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U43" s="3"/>
       <c r="V43" s="3"/>
-    </row>
-    <row r="44" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W43" s="14"/>
+      <c r="X43" s="14"/>
+      <c r="Y43" s="14"/>
+    </row>
+    <row r="44" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="13"/>
       <c r="G44" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
       <c r="M44" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
+      <c r="P44" s="13"/>
+      <c r="Q44" s="13"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
       <c r="T44" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U44" s="3"/>
       <c r="V44" s="3"/>
-    </row>
-    <row r="45" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W44" s="14"/>
+      <c r="X44" s="14"/>
+      <c r="Y44" s="14"/>
+    </row>
+    <row r="45" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="13"/>
       <c r="G45" s="1"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
       <c r="M45" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
+      <c r="P45" s="13"/>
+      <c r="Q45" s="13"/>
+      <c r="R45" s="14"/>
+      <c r="S45" s="14"/>
       <c r="T45" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="U45" s="3"/>
       <c r="V45" s="3"/>
-    </row>
-    <row r="46" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W45" s="14"/>
+      <c r="X45" s="14"/>
+      <c r="Y45" s="14"/>
+    </row>
+    <row r="46" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="13"/>
       <c r="G46" s="1"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
       <c r="M46" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="13"/>
+      <c r="R46" s="14"/>
+      <c r="S46" s="14"/>
       <c r="T46" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U46" s="3"/>
       <c r="V46" s="3"/>
-    </row>
-    <row r="47" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W46" s="14"/>
+      <c r="X46" s="14"/>
+      <c r="Y46" s="14"/>
+    </row>
+    <row r="47" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="13"/>
       <c r="G47" s="2"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
       <c r="M47" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N47" s="3"/>
       <c r="O47" s="3"/>
+      <c r="P47" s="13"/>
+      <c r="Q47" s="13"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="14"/>
       <c r="T47" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U47" s="3"/>
       <c r="V47" s="3"/>
-    </row>
-    <row r="48" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W47" s="14"/>
+      <c r="X47" s="14"/>
+      <c r="Y47" s="14"/>
+    </row>
+    <row r="48" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="13"/>
       <c r="G48" s="2"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
       <c r="M48" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
+      <c r="P48" s="13"/>
+      <c r="Q48" s="13"/>
+      <c r="R48" s="14"/>
+      <c r="S48" s="14"/>
       <c r="T48" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U48" s="3"/>
       <c r="V48" s="3"/>
-    </row>
-    <row r="49" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W48" s="14"/>
+      <c r="X48" s="14"/>
+      <c r="Y48" s="14"/>
+    </row>
+    <row r="49" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="13"/>
       <c r="G49" s="1"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
       <c r="M49" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N49" s="3"/>
       <c r="O49" s="3"/>
+      <c r="P49" s="13"/>
+      <c r="Q49" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="R49" s="18"/>
+      <c r="S49" s="14"/>
       <c r="T49" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U49" s="3"/>
       <c r="V49" s="3"/>
-    </row>
-    <row r="50" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W49" s="14"/>
+      <c r="X49" s="14"/>
+      <c r="Y49" s="14"/>
+    </row>
+    <row r="50" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="13"/>
       <c r="G50" s="1"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
       <c r="M50" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
+      <c r="P50" s="13"/>
+      <c r="Q50" s="18"/>
+      <c r="R50" s="18"/>
+      <c r="S50" s="14"/>
       <c r="T50" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U50" s="3"/>
       <c r="V50" s="3"/>
-    </row>
-    <row r="51" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W50" s="14"/>
+      <c r="X50" s="14"/>
+      <c r="Y50" s="14"/>
+    </row>
+    <row r="51" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13"/>
       <c r="M51" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
+      <c r="P51" s="13"/>
+      <c r="Q51" s="18"/>
+      <c r="R51" s="18"/>
+      <c r="S51" s="14"/>
       <c r="T51" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="U51" s="3"/>
       <c r="V51" s="3"/>
-    </row>
-    <row r="52" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W51" s="14"/>
+      <c r="X51" s="14"/>
+      <c r="Y51" s="14"/>
+    </row>
+    <row r="52" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="13"/>
       <c r="M52" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N52" s="3"/>
       <c r="O52" s="3"/>
+      <c r="P52" s="13"/>
+      <c r="Q52" s="18"/>
+      <c r="R52" s="18"/>
+      <c r="S52" s="14"/>
       <c r="T52" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U52" s="3"/>
       <c r="V52" s="3"/>
-    </row>
-    <row r="53" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W52" s="14"/>
+      <c r="X52" s="14"/>
+      <c r="Y52" s="14"/>
+    </row>
+    <row r="53" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="A53" s="12"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="13"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="13"/>
       <c r="M53" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
+      <c r="P53" s="13"/>
+      <c r="Q53" s="18"/>
+      <c r="R53" s="18"/>
+      <c r="S53" s="14"/>
       <c r="T53" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U53" s="3"/>
       <c r="V53" s="3"/>
-    </row>
-    <row r="54" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W53" s="14"/>
+      <c r="X53" s="14"/>
+      <c r="Y53" s="14"/>
+    </row>
+    <row r="54" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="13"/>
+      <c r="K54" s="13"/>
+      <c r="L54" s="13"/>
+      <c r="M54" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C54" s="1"/>
-      <c r="M54" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="N54" s="3"/>
       <c r="O54" s="3"/>
+      <c r="P54" s="13"/>
+      <c r="Q54" s="18"/>
+      <c r="R54" s="18"/>
+      <c r="S54" s="14"/>
       <c r="T54" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U54" s="3"/>
       <c r="V54" s="3"/>
-    </row>
-    <row r="55" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W54" s="14"/>
+      <c r="X54" s="14"/>
+      <c r="Y54" s="14"/>
+    </row>
+    <row r="55" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B55" s="1">
         <v>100000</v>
       </c>
       <c r="C55" s="1"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13"/>
+      <c r="L55" s="13"/>
       <c r="M55" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N55" s="3"/>
       <c r="O55" s="3"/>
+      <c r="P55" s="13"/>
+      <c r="Q55" s="13"/>
+      <c r="R55" s="14"/>
+      <c r="S55" s="14"/>
       <c r="T55" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="U55" s="3"/>
       <c r="V55" s="3"/>
-    </row>
-    <row r="56" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W55" s="14"/>
+      <c r="X55" s="14"/>
+      <c r="Y55" s="14"/>
+    </row>
+    <row r="56" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B56" s="1">
         <v>1</v>
       </c>
       <c r="C56" s="1"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
+      <c r="L56" s="13"/>
       <c r="M56" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N56" s="3"/>
       <c r="O56" s="3"/>
+      <c r="P56" s="13"/>
+      <c r="Q56" s="13"/>
+      <c r="R56" s="14"/>
+      <c r="S56" s="14"/>
       <c r="T56" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U56" s="3"/>
       <c r="V56" s="3"/>
-    </row>
-    <row r="57" spans="1:22" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="M57" s="4"/>
-    </row>
-    <row r="58" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W56" s="14"/>
+      <c r="X56" s="14"/>
+      <c r="Y56" s="14"/>
+    </row>
+    <row r="57" spans="1:25" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="14"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="13"/>
+      <c r="K57" s="13"/>
+      <c r="L57" s="13"/>
+      <c r="M57" s="13"/>
+      <c r="N57" s="13"/>
+      <c r="O57" s="13"/>
+      <c r="P57" s="13"/>
+      <c r="Q57" s="13"/>
+      <c r="R57" s="14"/>
+      <c r="S57" s="14"/>
+      <c r="T57" s="14"/>
+      <c r="U57" s="14"/>
+      <c r="V57" s="14"/>
+      <c r="W57" s="14"/>
+      <c r="X57" s="14"/>
+      <c r="Y57" s="14"/>
+    </row>
+    <row r="58" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13"/>
+      <c r="K58" s="13"/>
+      <c r="L58" s="13"/>
+      <c r="M58" s="13"/>
+      <c r="N58" s="13"/>
+      <c r="O58" s="13"/>
+      <c r="P58" s="13"/>
+      <c r="Q58" s="13"/>
+      <c r="R58" s="14"/>
+      <c r="S58" s="14"/>
+      <c r="T58" s="14"/>
+      <c r="U58" s="14"/>
+      <c r="V58" s="14"/>
+      <c r="W58" s="14"/>
+      <c r="X58" s="14"/>
+      <c r="Y58" s="14"/>
+    </row>
+    <row r="59" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M58" s="4"/>
-    </row>
-    <row r="59" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="B59" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C59" s="3">
         <v>80000</v>
       </c>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="13"/>
+      <c r="K59" s="13"/>
+      <c r="L59" s="13"/>
       <c r="M59" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O59" s="1"/>
+      <c r="P59" s="13"/>
+      <c r="Q59" s="13"/>
+      <c r="R59" s="14"/>
+      <c r="S59" s="14"/>
       <c r="T59" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U59" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="V59" s="1"/>
-    </row>
-    <row r="60" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W59" s="14"/>
+      <c r="X59" s="14"/>
+      <c r="Y59" s="14"/>
+    </row>
+    <row r="60" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="13"/>
+      <c r="K60" s="13"/>
+      <c r="L60" s="13"/>
       <c r="M60" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N60" s="1">
         <v>5000</v>
       </c>
       <c r="O60" s="1"/>
+      <c r="P60" s="13"/>
+      <c r="Q60" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="R60" s="18"/>
+      <c r="S60" s="14"/>
       <c r="T60" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U60" s="1">
         <v>5000</v>
       </c>
       <c r="V60" s="1"/>
-    </row>
-    <row r="61" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W60" s="14"/>
+      <c r="X60" s="14"/>
+      <c r="Y60" s="14"/>
+    </row>
+    <row r="61" spans="1:25" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="13"/>
+      <c r="L61" s="13"/>
       <c r="M61" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N61" s="1">
         <v>3</v>
       </c>
       <c r="O61" s="1"/>
+      <c r="P61" s="13"/>
+      <c r="Q61" s="18"/>
+      <c r="R61" s="18"/>
+      <c r="S61" s="14"/>
       <c r="T61" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U61" s="1">
         <v>3</v>
       </c>
       <c r="V61" s="1"/>
-    </row>
-    <row r="62" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W61" s="14"/>
+      <c r="X61" s="14"/>
+      <c r="Y61" s="14"/>
+    </row>
+    <row r="62" spans="1:25" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
-      <c r="U62" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="63" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="13"/>
+      <c r="K62" s="13"/>
+      <c r="L62" s="13"/>
+      <c r="M62" s="13"/>
+      <c r="N62" s="13"/>
+      <c r="O62" s="13"/>
+      <c r="P62" s="13"/>
+      <c r="Q62" s="18"/>
+      <c r="R62" s="18"/>
+      <c r="S62" s="14"/>
+      <c r="T62" s="14"/>
+      <c r="U62" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="V62" s="14"/>
+      <c r="W62" s="14"/>
+      <c r="X62" s="14"/>
+      <c r="Y62" s="14"/>
+    </row>
+    <row r="63" spans="1:25" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="13"/>
+      <c r="L63" s="13"/>
       <c r="M63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N63" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N63" s="1" t="s">
+      <c r="O63" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O63" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="P63" s="13"/>
+      <c r="Q63" s="18"/>
+      <c r="R63" s="18"/>
+      <c r="S63" s="14"/>
       <c r="T63" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="U63" s="10" t="s">
-        <v>54</v>
+        <v>7</v>
+      </c>
+      <c r="U63" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="V63" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="W63" s="14"/>
+      <c r="X63" s="14"/>
+      <c r="Y63" s="14"/>
+    </row>
+    <row r="64" spans="1:25" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="13"/>
+      <c r="K64" s="13"/>
+      <c r="L64" s="13"/>
       <c r="M64" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N64" s="3"/>
       <c r="O64" s="3"/>
+      <c r="P64" s="13"/>
+      <c r="Q64" s="18"/>
+      <c r="R64" s="18"/>
+      <c r="S64" s="14"/>
       <c r="T64" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U64" s="3"/>
       <c r="V64" s="3"/>
-    </row>
-    <row r="65" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W64" s="14"/>
+      <c r="X64" s="14"/>
+      <c r="Y64" s="14"/>
+    </row>
+    <row r="65" spans="1:25" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="13"/>
+      <c r="K65" s="13"/>
+      <c r="L65" s="13"/>
       <c r="M65" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N65" s="3"/>
       <c r="O65" s="3"/>
+      <c r="P65" s="13"/>
+      <c r="Q65" s="18"/>
+      <c r="R65" s="18"/>
+      <c r="S65" s="14"/>
       <c r="T65" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U65" s="3"/>
       <c r="V65" s="3"/>
-    </row>
-    <row r="66" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W65" s="14"/>
+      <c r="X65" s="14"/>
+      <c r="Y65" s="14"/>
+    </row>
+    <row r="66" spans="1:25" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="13"/>
+      <c r="K66" s="13"/>
+      <c r="L66" s="13"/>
       <c r="M66" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N66" s="3"/>
       <c r="O66" s="3"/>
+      <c r="P66" s="13"/>
+      <c r="Q66" s="13"/>
+      <c r="R66" s="14"/>
+      <c r="S66" s="14"/>
       <c r="T66" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U66" s="3"/>
       <c r="V66" s="3"/>
-    </row>
-    <row r="67" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W66" s="14"/>
+      <c r="X66" s="14"/>
+      <c r="Y66" s="14"/>
+    </row>
+    <row r="67" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="13"/>
       <c r="M67" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N67" s="3"/>
       <c r="O67" s="3"/>
+      <c r="P67" s="13"/>
+      <c r="Q67" s="13"/>
+      <c r="R67" s="14"/>
+      <c r="S67" s="14"/>
       <c r="T67" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U67" s="3"/>
       <c r="V67" s="3"/>
-    </row>
-    <row r="68" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W67" s="14"/>
+      <c r="X67" s="14"/>
+      <c r="Y67" s="14"/>
+    </row>
+    <row r="68" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="13"/>
+      <c r="K68" s="13"/>
+      <c r="L68" s="13"/>
       <c r="M68" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N68" s="3"/>
       <c r="O68" s="3"/>
+      <c r="P68" s="13"/>
+      <c r="Q68" s="13"/>
+      <c r="R68" s="14"/>
+      <c r="S68" s="14"/>
       <c r="T68" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U68" s="3"/>
       <c r="V68" s="3"/>
-    </row>
-    <row r="69" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W68" s="14"/>
+      <c r="X68" s="14"/>
+      <c r="Y68" s="14"/>
+    </row>
+    <row r="69" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="13"/>
+      <c r="K69" s="13"/>
+      <c r="L69" s="13"/>
       <c r="M69" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N69" s="3"/>
       <c r="O69" s="3"/>
+      <c r="P69" s="13"/>
+      <c r="Q69" s="13"/>
+      <c r="R69" s="14"/>
+      <c r="S69" s="14"/>
       <c r="T69" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U69" s="3"/>
       <c r="V69" s="3"/>
-    </row>
-    <row r="70" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W69" s="14"/>
+      <c r="X69" s="14"/>
+      <c r="Y69" s="14"/>
+    </row>
+    <row r="70" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="13"/>
+      <c r="K70" s="13"/>
+      <c r="L70" s="13"/>
       <c r="M70" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N70" s="3"/>
       <c r="O70" s="3"/>
+      <c r="P70" s="13"/>
+      <c r="Q70" s="13"/>
+      <c r="R70" s="14"/>
+      <c r="S70" s="14"/>
       <c r="T70" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U70" s="3"/>
       <c r="V70" s="3"/>
-    </row>
-    <row r="71" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W70" s="14"/>
+      <c r="X70" s="14"/>
+      <c r="Y70" s="14"/>
+    </row>
+    <row r="71" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
+      <c r="H71" s="13"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="13"/>
+      <c r="K71" s="13"/>
+      <c r="L71" s="13"/>
       <c r="M71" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N71" s="3"/>
       <c r="O71" s="3"/>
+      <c r="P71" s="13"/>
+      <c r="Q71" s="13"/>
+      <c r="R71" s="14"/>
+      <c r="S71" s="14"/>
       <c r="T71" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U71" s="3"/>
       <c r="V71" s="3"/>
-    </row>
-    <row r="72" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W71" s="14"/>
+      <c r="X71" s="14"/>
+      <c r="Y71" s="14"/>
+    </row>
+    <row r="72" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="13"/>
+      <c r="I72" s="13"/>
+      <c r="J72" s="13"/>
+      <c r="K72" s="13"/>
+      <c r="L72" s="13"/>
       <c r="M72" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N72" s="3"/>
       <c r="O72" s="3"/>
+      <c r="P72" s="13"/>
+      <c r="Q72" s="13"/>
+      <c r="R72" s="14"/>
+      <c r="S72" s="14"/>
       <c r="T72" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U72" s="3"/>
       <c r="V72" s="3"/>
-    </row>
-    <row r="73" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W72" s="14"/>
+      <c r="X72" s="14"/>
+      <c r="Y72" s="14"/>
+    </row>
+    <row r="73" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="13"/>
+      <c r="K73" s="13"/>
+      <c r="L73" s="13"/>
       <c r="M73" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N73" s="3"/>
       <c r="O73" s="3"/>
+      <c r="P73" s="13"/>
+      <c r="Q73" s="13"/>
+      <c r="R73" s="14"/>
+      <c r="S73" s="14"/>
       <c r="T73" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U73" s="3"/>
       <c r="V73" s="3"/>
-    </row>
-    <row r="74" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W73" s="14"/>
+      <c r="X73" s="14"/>
+      <c r="Y73" s="14"/>
+    </row>
+    <row r="74" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="13"/>
+      <c r="J74" s="13"/>
+      <c r="K74" s="13"/>
+      <c r="L74" s="13"/>
       <c r="M74" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N74" s="3"/>
       <c r="O74" s="3"/>
+      <c r="P74" s="13"/>
+      <c r="Q74" s="13"/>
+      <c r="R74" s="14"/>
+      <c r="S74" s="14"/>
       <c r="T74" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U74" s="3"/>
       <c r="V74" s="3"/>
-    </row>
-    <row r="75" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W74" s="14"/>
+      <c r="X74" s="14"/>
+      <c r="Y74" s="14"/>
+    </row>
+    <row r="75" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="13"/>
+      <c r="K75" s="13"/>
+      <c r="L75" s="13"/>
       <c r="M75" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N75" s="3"/>
       <c r="O75" s="3"/>
+      <c r="P75" s="13"/>
+      <c r="Q75" s="13"/>
+      <c r="R75" s="14"/>
+      <c r="S75" s="14"/>
       <c r="T75" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U75" s="3"/>
       <c r="V75" s="3"/>
-    </row>
-    <row r="76" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W75" s="14"/>
+      <c r="X75" s="14"/>
+      <c r="Y75" s="14"/>
+    </row>
+    <row r="76" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="13"/>
+      <c r="K76" s="13"/>
+      <c r="L76" s="13"/>
       <c r="M76" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N76" s="3"/>
       <c r="O76" s="3"/>
+      <c r="P76" s="13"/>
+      <c r="Q76" s="13"/>
+      <c r="R76" s="14"/>
+      <c r="S76" s="14"/>
       <c r="T76" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="U76" s="3"/>
       <c r="V76" s="3"/>
-    </row>
-    <row r="77" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W76" s="14"/>
+      <c r="X76" s="14"/>
+      <c r="Y76" s="14"/>
+    </row>
+    <row r="77" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="A77" s="12"/>
+      <c r="B77" s="12"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="13"/>
+      <c r="K77" s="13"/>
+      <c r="L77" s="13"/>
       <c r="M77" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N77" s="3"/>
       <c r="O77" s="3"/>
+      <c r="P77" s="13"/>
+      <c r="Q77" s="13"/>
+      <c r="R77" s="14"/>
+      <c r="S77" s="14"/>
       <c r="T77" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U77" s="3"/>
       <c r="V77" s="3"/>
-    </row>
-    <row r="78" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W77" s="14"/>
+      <c r="X77" s="14"/>
+      <c r="Y77" s="14"/>
+    </row>
+    <row r="78" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="A78" s="12"/>
+      <c r="B78" s="12"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="13"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="13"/>
+      <c r="J78" s="13"/>
+      <c r="K78" s="13"/>
+      <c r="L78" s="13"/>
       <c r="M78" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N78" s="3"/>
       <c r="O78" s="3"/>
+      <c r="P78" s="13"/>
+      <c r="Q78" s="13"/>
+      <c r="R78" s="14"/>
+      <c r="S78" s="14"/>
       <c r="T78" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U78" s="3"/>
       <c r="V78" s="3"/>
-    </row>
-    <row r="79" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W78" s="14"/>
+      <c r="X78" s="14"/>
+      <c r="Y78" s="14"/>
+    </row>
+    <row r="79" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="A79" s="12"/>
+      <c r="B79" s="12"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="13"/>
+      <c r="I79" s="13"/>
+      <c r="J79" s="13"/>
+      <c r="K79" s="13"/>
+      <c r="L79" s="13"/>
       <c r="M79" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N79" s="3"/>
       <c r="O79" s="3"/>
+      <c r="P79" s="13"/>
+      <c r="Q79" s="13"/>
+      <c r="R79" s="14"/>
+      <c r="S79" s="14"/>
       <c r="T79" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U79" s="3"/>
       <c r="V79" s="3"/>
-    </row>
-    <row r="80" spans="1:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W79" s="14"/>
+      <c r="X79" s="14"/>
+      <c r="Y79" s="14"/>
+    </row>
+    <row r="80" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="A80" s="12"/>
+      <c r="B80" s="12"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="13"/>
+      <c r="I80" s="13"/>
+      <c r="J80" s="13"/>
+      <c r="K80" s="13"/>
+      <c r="L80" s="13"/>
       <c r="M80" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N80" s="3"/>
       <c r="O80" s="3"/>
+      <c r="P80" s="13"/>
+      <c r="Q80" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="R80" s="18"/>
+      <c r="S80" s="14"/>
       <c r="T80" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U80" s="3"/>
       <c r="V80" s="3"/>
-    </row>
-    <row r="81" spans="13:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W80" s="14"/>
+      <c r="X80" s="14"/>
+      <c r="Y80" s="14"/>
+    </row>
+    <row r="81" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="A81" s="12"/>
+      <c r="B81" s="12"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="13"/>
+      <c r="J81" s="13"/>
+      <c r="K81" s="13"/>
+      <c r="L81" s="13"/>
       <c r="M81" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N81" s="3"/>
       <c r="O81" s="3"/>
+      <c r="P81" s="13"/>
+      <c r="Q81" s="18"/>
+      <c r="R81" s="18"/>
+      <c r="S81" s="14"/>
       <c r="T81" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U81" s="3"/>
       <c r="V81" s="3"/>
-    </row>
-    <row r="82" spans="13:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W81" s="14"/>
+      <c r="X81" s="14"/>
+      <c r="Y81" s="14"/>
+    </row>
+    <row r="82" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="A82" s="14"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="14"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="13"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="13"/>
+      <c r="I82" s="13"/>
+      <c r="J82" s="13"/>
+      <c r="K82" s="13"/>
+      <c r="L82" s="13"/>
       <c r="M82" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N82" s="3"/>
       <c r="O82" s="3"/>
+      <c r="P82" s="13"/>
+      <c r="Q82" s="18"/>
+      <c r="R82" s="18"/>
+      <c r="S82" s="14"/>
       <c r="T82" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="U82" s="3"/>
       <c r="V82" s="3"/>
-    </row>
-    <row r="83" spans="13:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W82" s="14"/>
+      <c r="X82" s="14"/>
+      <c r="Y82" s="14"/>
+    </row>
+    <row r="83" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="A83" s="14"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13"/>
+      <c r="I83" s="13"/>
+      <c r="J83" s="13"/>
+      <c r="K83" s="13"/>
+      <c r="L83" s="13"/>
       <c r="M83" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N83" s="3"/>
       <c r="O83" s="3"/>
+      <c r="P83" s="13"/>
+      <c r="Q83" s="18"/>
+      <c r="R83" s="18"/>
+      <c r="S83" s="14"/>
       <c r="T83" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U83" s="3"/>
       <c r="V83" s="3"/>
-    </row>
-    <row r="84" spans="13:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W83" s="14"/>
+      <c r="X83" s="14"/>
+      <c r="Y83" s="14"/>
+    </row>
+    <row r="84" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="A84" s="14"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="14"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="13"/>
+      <c r="J84" s="13"/>
+      <c r="K84" s="13"/>
+      <c r="L84" s="13"/>
       <c r="M84" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N84" s="3"/>
       <c r="O84" s="3"/>
+      <c r="P84" s="13"/>
+      <c r="Q84" s="18"/>
+      <c r="R84" s="18"/>
+      <c r="S84" s="14"/>
       <c r="T84" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U84" s="3"/>
       <c r="V84" s="3"/>
-    </row>
-    <row r="85" spans="13:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W84" s="14"/>
+      <c r="X84" s="14"/>
+      <c r="Y84" s="14"/>
+    </row>
+    <row r="85" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="A85" s="14"/>
+      <c r="B85" s="14"/>
+      <c r="C85" s="14"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="13"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="13"/>
+      <c r="K85" s="13"/>
+      <c r="L85" s="13"/>
       <c r="M85" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N85" s="3"/>
       <c r="O85" s="3"/>
+      <c r="P85" s="13"/>
+      <c r="Q85" s="18"/>
+      <c r="R85" s="18"/>
+      <c r="S85" s="14"/>
       <c r="T85" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U85" s="3"/>
       <c r="V85" s="3"/>
-    </row>
-    <row r="86" spans="13:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W85" s="14"/>
+      <c r="X85" s="14"/>
+      <c r="Y85" s="14"/>
+    </row>
+    <row r="86" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="A86" s="14"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="13"/>
+      <c r="G86" s="13"/>
+      <c r="H86" s="13"/>
+      <c r="I86" s="13"/>
+      <c r="J86" s="13"/>
+      <c r="K86" s="13"/>
+      <c r="L86" s="13"/>
       <c r="M86" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N86" s="3"/>
       <c r="O86" s="3"/>
+      <c r="P86" s="13"/>
+      <c r="Q86" s="13"/>
+      <c r="R86" s="14"/>
+      <c r="S86" s="14"/>
       <c r="T86" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="U86" s="3"/>
       <c r="V86" s="3"/>
-    </row>
-    <row r="87" spans="13:22" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="W86" s="14"/>
+      <c r="X86" s="14"/>
+      <c r="Y86" s="14"/>
+    </row>
+    <row r="87" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="A87" s="14"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="14"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="13"/>
+      <c r="G87" s="13"/>
+      <c r="H87" s="13"/>
+      <c r="I87" s="13"/>
+      <c r="J87" s="13"/>
+      <c r="K87" s="13"/>
+      <c r="L87" s="13"/>
       <c r="M87" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N87" s="3"/>
       <c r="O87" s="3"/>
+      <c r="P87" s="13"/>
+      <c r="Q87" s="13"/>
+      <c r="R87" s="14"/>
+      <c r="S87" s="14"/>
       <c r="T87" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U87" s="3"/>
       <c r="V87" s="3"/>
-    </row>
-    <row r="88" spans="13:22" ht="12.65" x14ac:dyDescent="0.3">
-      <c r="M88" s="5"/>
-    </row>
-    <row r="89" spans="13:22" ht="12.65" x14ac:dyDescent="0.3"/>
-    <row r="90" spans="13:22" ht="12.65" x14ac:dyDescent="0.3"/>
-    <row r="91" spans="13:22" ht="12.65" x14ac:dyDescent="0.3"/>
-    <row r="92" spans="13:22" ht="12.65" x14ac:dyDescent="0.3"/>
-    <row r="93" spans="13:22" ht="12.65" x14ac:dyDescent="0.3"/>
-    <row r="94" spans="13:22" ht="12.65" x14ac:dyDescent="0.3"/>
-    <row r="95" spans="13:22" ht="12.65" x14ac:dyDescent="0.3"/>
-    <row r="96" spans="13:22" ht="12.65" x14ac:dyDescent="0.3"/>
+      <c r="W87" s="14"/>
+      <c r="X87" s="14"/>
+      <c r="Y87" s="14"/>
+    </row>
+    <row r="88" spans="1:25" ht="12.65" x14ac:dyDescent="0.3">
+      <c r="M88" s="4"/>
+    </row>
+    <row r="89" spans="1:25" ht="12.65" x14ac:dyDescent="0.3"/>
+    <row r="90" spans="1:25" ht="12.65" x14ac:dyDescent="0.3"/>
+    <row r="91" spans="1:25" ht="12.65" x14ac:dyDescent="0.3"/>
+    <row r="92" spans="1:25" ht="12.65" x14ac:dyDescent="0.3"/>
+    <row r="93" spans="1:25" ht="12.65" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="1:25" ht="12.65" x14ac:dyDescent="0.3"/>
+    <row r="95" spans="1:25" ht="12.65" x14ac:dyDescent="0.3"/>
+    <row r="96" spans="1:25" ht="12.65" x14ac:dyDescent="0.3"/>
     <row r="97" ht="12.65" x14ac:dyDescent="0.3"/>
     <row r="98" ht="12.65" x14ac:dyDescent="0.3"/>
     <row r="99" ht="12.65" x14ac:dyDescent="0.3"/>
@@ -2669,14 +4059,21 @@
     <row r="138" spans="7:7" ht="12.65" x14ac:dyDescent="0.3"/>
     <row r="139" spans="7:7" ht="12.65" x14ac:dyDescent="0.3"/>
     <row r="140" spans="7:7" ht="12.65" x14ac:dyDescent="0.3">
-      <c r="G140" s="5"/>
+      <c r="G140" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="11">
+    <mergeCell ref="Q80:R85"/>
+    <mergeCell ref="Q31:R36"/>
+    <mergeCell ref="Q25:R30"/>
+    <mergeCell ref="Q49:R54"/>
+    <mergeCell ref="Q60:R65"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="T2:V2"/>
+    <mergeCell ref="H1:N1"/>
+    <mergeCell ref="S1:X1"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>